<commit_message>
more tc and rollback
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\BankAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A69A51-F5DE-4BFC-92A4-A9E10F2EE018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F2F3F0-44D1-44A5-A61B-9BE219199ED4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="57">
   <si>
     <t>Username</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Monthly</t>
+  </si>
+  <si>
+    <t>Kient@#!@#</t>
+  </si>
+  <si>
+    <t>Kientpt OR 1 = 1</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +618,28 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1131,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5841FF3-E4C8-45B8-BA97-62D3A09BBE5C}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>